<commit_message>
Added visualizer and network visualization methods
</commit_message>
<xml_diff>
--- a/data/input/SimulatorScenarios.xlsx
+++ b/data/input/SimulatorScenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20392"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/ABM4ALL/CovidNetworkContagion/data/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Developing\MelodieProject\CovidNetworkContagionVisual\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508B5DAD-8476-A548-9A5F-F27A1723DA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB5D11F-0873-4A58-9388-78F682C747F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="765" windowWidth="30240" windowHeight="17355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simulator_scenarios" sheetId="1" r:id="rId1"/>
@@ -65,18 +65,24 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -105,7 +111,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -381,20 +387,20 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.125" customWidth="1"/>
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.625" customWidth="1"/>
     <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.625" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="23.5" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -443,7 +449,7 @@
         <v>100</v>
       </c>
       <c r="D2">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>
@@ -478,7 +484,7 @@
         <v>100</v>
       </c>
       <c r="D3">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
@@ -503,7 +509,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>